<commit_message>
Added reindexing for monoclinic
</commit_message>
<xml_diff>
--- a/data/SpacegroupGroups.xlsx
+++ b/data/SpacegroupGroups.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DWMoreau/MLI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0C9CCD-173C-A54C-94B6-2E563125C98C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921F8978-0E53-9042-9C0E-DDFF8AF22CCE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="2200" windowWidth="18860" windowHeight="14720" activeTab="2" xr2:uid="{858AA173-3D70-D14E-A9ED-F265E8D33CB5}"/>
+    <workbookView xWindow="1800" yWindow="880" windowWidth="25300" windowHeight="17800" xr2:uid="{858AA173-3D70-D14E-A9ED-F265E8D33CB5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Orthorhombic Groups" sheetId="5" r:id="rId1"/>
-    <sheet name="Cubic" sheetId="8" r:id="rId2"/>
-    <sheet name="Tetragonal" sheetId="9" r:id="rId3"/>
-    <sheet name="oC Reindex" sheetId="6" r:id="rId4"/>
-    <sheet name="oI" sheetId="2" r:id="rId5"/>
-    <sheet name="oF" sheetId="1" r:id="rId6"/>
-    <sheet name="oP" sheetId="4" r:id="rId7"/>
-    <sheet name="oC" sheetId="3" r:id="rId8"/>
-    <sheet name="oP reindex" sheetId="7" r:id="rId9"/>
+    <sheet name="Monoclinic, beta" sheetId="10" r:id="rId1"/>
+    <sheet name="Orthorhombic Groups" sheetId="5" r:id="rId2"/>
+    <sheet name="Cubic" sheetId="8" r:id="rId3"/>
+    <sheet name="Tetragonal" sheetId="9" r:id="rId4"/>
+    <sheet name="oC Reindex" sheetId="6" r:id="rId5"/>
+    <sheet name="oI" sheetId="2" r:id="rId6"/>
+    <sheet name="oF" sheetId="1" r:id="rId7"/>
+    <sheet name="oP" sheetId="4" r:id="rId8"/>
+    <sheet name="oC" sheetId="3" r:id="rId9"/>
+    <sheet name="oP reindex" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3942" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4552" uniqueCount="390">
   <si>
     <t>F222</t>
   </si>
@@ -1041,6 +1042,168 @@
   </si>
   <si>
     <t>96, 92</t>
+  </si>
+  <si>
+    <t>P 1 2 1, P 1 m 1, P 1 2/m 1</t>
+  </si>
+  <si>
+    <t>3, 6, 10</t>
+  </si>
+  <si>
+    <t>P 1 21 1, P 1 21/m 1</t>
+  </si>
+  <si>
+    <t>4, 11</t>
+  </si>
+  <si>
+    <t>P 1 c 1, P 1 2/c 1</t>
+  </si>
+  <si>
+    <t>7, 13</t>
+  </si>
+  <si>
+    <t>P 1 a 1, P 1 2/a 1</t>
+  </si>
+  <si>
+    <t>P 1 n 1, P 1 2/n 1</t>
+  </si>
+  <si>
+    <t>P 1 21/c 1</t>
+  </si>
+  <si>
+    <t>P 1 21/a 1</t>
+  </si>
+  <si>
+    <t>P 1 21/n 1</t>
+  </si>
+  <si>
+    <t>h + l = 4n</t>
+  </si>
+  <si>
+    <t>B 1 2 1, B 1 m 1, B 1 2/m 1</t>
+  </si>
+  <si>
+    <t>B 1 21 1, B 1 21/m 1</t>
+  </si>
+  <si>
+    <t>B 1 a 1, B 1 2/a 1</t>
+  </si>
+  <si>
+    <t>B 1 a 1, B 1 2/d 1</t>
+  </si>
+  <si>
+    <t>B 1 21/d 1</t>
+  </si>
+  <si>
+    <t>A 1 2 1, A 1 m 1, A 1 2/m 1</t>
+  </si>
+  <si>
+    <t>5, 8, 12</t>
+  </si>
+  <si>
+    <t>A 1 a 1, A 1 2/a 1</t>
+  </si>
+  <si>
+    <t>9, 15</t>
+  </si>
+  <si>
+    <t>C 1 2 1, C 1 m 1, C 1 2/m 1</t>
+  </si>
+  <si>
+    <t>C 1 c 1, C 1 2/c 1</t>
+  </si>
+  <si>
+    <t>I 1 2 1, I 1 m 1, I 1 2/m 1</t>
+  </si>
+  <si>
+    <t>I 1 a 1, I 1 2/a 1</t>
+  </si>
+  <si>
+    <t>h + k, h + l, k + l = 2n</t>
+  </si>
+  <si>
+    <t>F 1 2 1, F 1 m 1, F 1 2/m 1</t>
+  </si>
+  <si>
+    <t>F 1 d 1, F 1 2/d 1</t>
+  </si>
+  <si>
+    <t>beta != 90</t>
+  </si>
+  <si>
+    <t>alpha != 90</t>
+  </si>
+  <si>
+    <t>P 1 1 2, P 1 1 m, P 1 1 2/m</t>
+  </si>
+  <si>
+    <t>P 1 1 21, P 1 1 21/m</t>
+  </si>
+  <si>
+    <t>P 1 1 a, P 1 1 2/a</t>
+  </si>
+  <si>
+    <t>P 1 1 b, P 1 1 2/b</t>
+  </si>
+  <si>
+    <t>P 1 1 n, P 1 1 2/n</t>
+  </si>
+  <si>
+    <t>P 1 1 21/a</t>
+  </si>
+  <si>
+    <t>P 1 1 21/b</t>
+  </si>
+  <si>
+    <t>P 1 1 21/n</t>
+  </si>
+  <si>
+    <t>B 1 1 2, B 1 1 m, B 1 1 2/m</t>
+  </si>
+  <si>
+    <t>B 1 1 b, B 1 1 2/b</t>
+  </si>
+  <si>
+    <t>h + k = 4n</t>
+  </si>
+  <si>
+    <t>C 1 1 2, C 1 1 m, B 1 1 2/m</t>
+  </si>
+  <si>
+    <t>C 1 1 21, C 1 1 21/m</t>
+  </si>
+  <si>
+    <t>A 1 1 2, A 1 1 m, C 1 2/m 1</t>
+  </si>
+  <si>
+    <t>A 1 1 a, A 1 2/a 1</t>
+  </si>
+  <si>
+    <t>I 1 1 2, I 1 1 m, I 1 1 2/m</t>
+  </si>
+  <si>
+    <t>I 1 1 a, I 1 1 2/a</t>
+  </si>
+  <si>
+    <t>F 1 1 2, F 1 1 m, F 1 1 2/m</t>
+  </si>
+  <si>
+    <t>F 1 1 d, F 1 1 2/d</t>
+  </si>
+  <si>
+    <t>C 1 1 d, C 1 1 2/d</t>
+  </si>
+  <si>
+    <t>C 1 1 21/d</t>
+  </si>
+  <si>
+    <t>C 1 1 21/a</t>
+  </si>
+  <si>
+    <t>C 1 1 a, C 1 1 2/a</t>
+  </si>
+  <si>
+    <t>7, 15</t>
   </si>
 </sst>
 </file>
@@ -1533,6 +1696,2930 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F97899-3E7B-2A4E-8106-D9711D155142}">
+  <dimension ref="A1:Q146"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D3" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>340</v>
+      </c>
+      <c r="D14" t="s">
+        <v>342</v>
+      </c>
+      <c r="G14" t="s">
+        <v>343</v>
+      </c>
+      <c r="J14" t="s">
+        <v>344</v>
+      </c>
+      <c r="M14" t="s">
+        <v>345</v>
+      </c>
+      <c r="P14" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>341</v>
+      </c>
+      <c r="D15" t="s">
+        <v>341</v>
+      </c>
+      <c r="G15" t="s">
+        <v>341</v>
+      </c>
+      <c r="J15">
+        <v>14</v>
+      </c>
+      <c r="M15">
+        <v>14</v>
+      </c>
+      <c r="P15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="J16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="M16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="P16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="3"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="J17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="M17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="P17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="3"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="J19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="M19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N19" s="3"/>
+      <c r="P19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="3"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="M20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="J21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="G22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="P22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>337</v>
+      </c>
+      <c r="D26" t="s">
+        <v>339</v>
+      </c>
+      <c r="G26" t="s">
+        <v>341</v>
+      </c>
+      <c r="J26" t="s">
+        <v>341</v>
+      </c>
+      <c r="M26">
+        <v>14</v>
+      </c>
+      <c r="P26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q31" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="3"/>
+      <c r="J32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K32" s="3"/>
+      <c r="M32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q32" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q33" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>354</v>
+      </c>
+      <c r="D36" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>354</v>
+      </c>
+      <c r="D46" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="D53" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>354</v>
+      </c>
+      <c r="D56" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>354</v>
+      </c>
+      <c r="D66" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="12" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>366</v>
+      </c>
+      <c r="D76" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>337</v>
+      </c>
+      <c r="D77" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B78" s="3"/>
+      <c r="D78" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="D79" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="D80" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B81" s="3"/>
+      <c r="D81" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E81" s="3"/>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" s="3"/>
+      <c r="D82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" s="3"/>
+      <c r="D83" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E83" s="3"/>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B84" s="3"/>
+      <c r="D84" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>369</v>
+      </c>
+      <c r="D87" t="s">
+        <v>368</v>
+      </c>
+      <c r="G87" t="s">
+        <v>370</v>
+      </c>
+      <c r="J87" t="s">
+        <v>372</v>
+      </c>
+      <c r="M87" t="s">
+        <v>371</v>
+      </c>
+      <c r="P87" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>341</v>
+      </c>
+      <c r="D88" t="s">
+        <v>341</v>
+      </c>
+      <c r="G88" t="s">
+        <v>341</v>
+      </c>
+      <c r="J88">
+        <v>14</v>
+      </c>
+      <c r="M88">
+        <v>14</v>
+      </c>
+      <c r="P88">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" s="3"/>
+      <c r="D89" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E89" s="3"/>
+      <c r="G89" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H89" s="3"/>
+      <c r="J89" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K89" s="3"/>
+      <c r="M89" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N89" s="3"/>
+      <c r="P89" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q89" s="3"/>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="3"/>
+      <c r="D90" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E90" s="3"/>
+      <c r="G90" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H90" s="3"/>
+      <c r="J90" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K90" s="3"/>
+      <c r="M90" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N90" s="3"/>
+      <c r="P90" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q90" s="3"/>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E91" s="3"/>
+      <c r="G91" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H91" s="3"/>
+      <c r="J91" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K91" s="3"/>
+      <c r="M91" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P91" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q91" s="3"/>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J92" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K92" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M92" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N92" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P92" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q92" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" s="3"/>
+      <c r="D93" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J93" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K93" s="3"/>
+      <c r="M93" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N93" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P93" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q93" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E94" s="3"/>
+      <c r="G94" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J94" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K94" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M94" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N94" s="3"/>
+      <c r="P94" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q94" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B95" s="3"/>
+      <c r="D95" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E95" s="3"/>
+      <c r="G95" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H95" s="3"/>
+      <c r="J95" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K95" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M95" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N95" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P95" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q95" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="J98" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="M98" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="P98" s="3" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>337</v>
+      </c>
+      <c r="D99" t="s">
+        <v>339</v>
+      </c>
+      <c r="G99" t="s">
+        <v>389</v>
+      </c>
+      <c r="J99" t="s">
+        <v>341</v>
+      </c>
+      <c r="M99">
+        <v>14</v>
+      </c>
+      <c r="P99">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J100" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K100" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M100" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N100" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P100" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q100" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H101" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J101" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K101" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M101" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N101" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P101" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q101" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J102" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K102" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M102" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N102" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P102" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q102" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H103" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J103" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K103" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="M103" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N103" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P103" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q103" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J104" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K104" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M104" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N104" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P104" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q104" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H105" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J105" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K105" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M105" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N105" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P105" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q105" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B106" s="3"/>
+      <c r="D106" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H106" s="3"/>
+      <c r="J106" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K106" s="3"/>
+      <c r="M106" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N106" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P106" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q106" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>354</v>
+      </c>
+      <c r="D109" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B115" s="3"/>
+      <c r="D115" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>354</v>
+      </c>
+      <c r="D119" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B124" s="3"/>
+      <c r="D124" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>354</v>
+      </c>
+      <c r="D129" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>354</v>
+      </c>
+      <c r="D139" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5FC088-8BF5-F647-8378-DF4EED211D72}">
+  <dimension ref="A1:Q41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J1" t="s">
+        <v>182</v>
+      </c>
+      <c r="K1" t="s">
+        <v>183</v>
+      </c>
+      <c r="M1" t="s">
+        <v>181</v>
+      </c>
+      <c r="N1" t="s">
+        <v>184</v>
+      </c>
+      <c r="P1" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="D2" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="G2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="J2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="M2" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="N2" s="8"/>
+      <c r="P2" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="D3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="G3" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="J3" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="M3" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="N3" s="8"/>
+      <c r="P3" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E8" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8" t="s">
+        <v>179</v>
+      </c>
+      <c r="H8" t="s">
+        <v>180</v>
+      </c>
+      <c r="J8" t="s">
+        <v>182</v>
+      </c>
+      <c r="K8" t="s">
+        <v>183</v>
+      </c>
+      <c r="M8" t="s">
+        <v>181</v>
+      </c>
+      <c r="N8" t="s">
+        <v>184</v>
+      </c>
+      <c r="P8" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="D9" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="G9" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="J9" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="D10" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="G10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="J10" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D15" t="s">
+        <v>177</v>
+      </c>
+      <c r="E15" t="s">
+        <v>178</v>
+      </c>
+      <c r="G15" t="s">
+        <v>179</v>
+      </c>
+      <c r="H15" t="s">
+        <v>180</v>
+      </c>
+      <c r="J15" t="s">
+        <v>182</v>
+      </c>
+      <c r="K15" t="s">
+        <v>183</v>
+      </c>
+      <c r="M15" t="s">
+        <v>181</v>
+      </c>
+      <c r="N15" t="s">
+        <v>184</v>
+      </c>
+      <c r="P15" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="D16" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="G16" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="J16" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="D17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="G17" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="J17" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>176</v>
+      </c>
+      <c r="D22" t="s">
+        <v>177</v>
+      </c>
+      <c r="E22" t="s">
+        <v>178</v>
+      </c>
+      <c r="G22" t="s">
+        <v>179</v>
+      </c>
+      <c r="H22" t="s">
+        <v>180</v>
+      </c>
+      <c r="J22" t="s">
+        <v>182</v>
+      </c>
+      <c r="K22" t="s">
+        <v>183</v>
+      </c>
+      <c r="M22" t="s">
+        <v>181</v>
+      </c>
+      <c r="N22" t="s">
+        <v>184</v>
+      </c>
+      <c r="P22" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="D23" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="G23" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="D24" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="G24" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30" s="8"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="8"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B37" s="5"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" s="5"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC84443B-7CEE-7745-A632-86C52473395D}">
   <dimension ref="A1:W164"/>
   <sheetViews>
@@ -4755,7 +7842,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3512D7-A514-8E4F-BD6D-507969E8403F}">
   <dimension ref="A1:N79"/>
   <sheetViews>
@@ -6055,12 +9142,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4622A5-4C0E-4742-B133-5329BFA95A67}">
   <dimension ref="A1:Q90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F11" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7870,7 +10957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2736027-0895-9340-BA5B-E91645FE7BDE}">
   <dimension ref="A1:Q74"/>
   <sheetViews>
@@ -9400,7 +12487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16070A50-6E9C-B54D-9FFF-B281826AC096}">
   <dimension ref="A1:H29"/>
   <sheetViews>
@@ -9869,7 +12956,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A43CFF8-4568-7A46-92D0-A1E20AF674F5}">
   <dimension ref="A1:H30"/>
   <sheetViews>
@@ -10189,7 +13276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A6E9374-DB17-5248-A2A2-DCDC0DB93DC4}">
   <dimension ref="A1:P255"/>
   <sheetViews>
@@ -14491,7 +17578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A07B9D3-5C67-AB41-9F60-D3C009703861}">
   <dimension ref="A1:J94"/>
   <sheetViews>
@@ -16127,711 +19214,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5FC088-8BF5-F647-8378-DF4EED211D72}">
-  <dimension ref="A1:Q41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E1" t="s">
-        <v>178</v>
-      </c>
-      <c r="G1" t="s">
-        <v>179</v>
-      </c>
-      <c r="H1" t="s">
-        <v>180</v>
-      </c>
-      <c r="J1" t="s">
-        <v>182</v>
-      </c>
-      <c r="K1" t="s">
-        <v>183</v>
-      </c>
-      <c r="M1" t="s">
-        <v>181</v>
-      </c>
-      <c r="N1" t="s">
-        <v>184</v>
-      </c>
-      <c r="P1" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="D2" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="G2" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="H2" s="6"/>
-      <c r="J2" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="M2" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="N2" s="8"/>
-      <c r="P2" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q2" s="3"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="D3" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="G3" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="J3" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="K3" s="5"/>
-      <c r="M3" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="N3" s="8"/>
-      <c r="P3" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q3" s="3"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>176</v>
-      </c>
-      <c r="D8" t="s">
-        <v>177</v>
-      </c>
-      <c r="E8" t="s">
-        <v>178</v>
-      </c>
-      <c r="G8" t="s">
-        <v>179</v>
-      </c>
-      <c r="H8" t="s">
-        <v>180</v>
-      </c>
-      <c r="J8" t="s">
-        <v>182</v>
-      </c>
-      <c r="K8" t="s">
-        <v>183</v>
-      </c>
-      <c r="M8" t="s">
-        <v>181</v>
-      </c>
-      <c r="N8" t="s">
-        <v>184</v>
-      </c>
-      <c r="P8" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="D9" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="G9" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="J9" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="D10" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="G10" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="J10" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="K10" s="8"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>176</v>
-      </c>
-      <c r="D15" t="s">
-        <v>177</v>
-      </c>
-      <c r="E15" t="s">
-        <v>178</v>
-      </c>
-      <c r="G15" t="s">
-        <v>179</v>
-      </c>
-      <c r="H15" t="s">
-        <v>180</v>
-      </c>
-      <c r="J15" t="s">
-        <v>182</v>
-      </c>
-      <c r="K15" t="s">
-        <v>183</v>
-      </c>
-      <c r="M15" t="s">
-        <v>181</v>
-      </c>
-      <c r="N15" t="s">
-        <v>184</v>
-      </c>
-      <c r="P15" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="D16" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="G16" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H16" s="8"/>
-      <c r="J16" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="D17" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="G17" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H17" s="8"/>
-      <c r="J17" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>176</v>
-      </c>
-      <c r="D22" t="s">
-        <v>177</v>
-      </c>
-      <c r="E22" t="s">
-        <v>178</v>
-      </c>
-      <c r="G22" t="s">
-        <v>179</v>
-      </c>
-      <c r="H22" t="s">
-        <v>180</v>
-      </c>
-      <c r="J22" t="s">
-        <v>182</v>
-      </c>
-      <c r="K22" t="s">
-        <v>183</v>
-      </c>
-      <c r="M22" t="s">
-        <v>181</v>
-      </c>
-      <c r="N22" t="s">
-        <v>184</v>
-      </c>
-      <c r="P22" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="D23" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="E23" s="6"/>
-      <c r="G23" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="D24" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="G24" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B30" s="8"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B31" s="8"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B37" s="5"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B38" s="5"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Edits to get monoclinic unit cell regression training
</commit_message>
<xml_diff>
--- a/data/SpacegroupGroups.xlsx
+++ b/data/SpacegroupGroups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DWMoreau/MLI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921F8978-0E53-9042-9C0E-DDFF8AF22CCE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1358C565-DB6D-3647-A900-FDF88719F503}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="880" windowWidth="25300" windowHeight="17800" xr2:uid="{858AA173-3D70-D14E-A9ED-F265E8D33CB5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4552" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4857" uniqueCount="414">
   <si>
     <t>F222</t>
   </si>
@@ -1089,9 +1089,6 @@
     <t>B 1 a 1, B 1 2/a 1</t>
   </si>
   <si>
-    <t>B 1 a 1, B 1 2/d 1</t>
-  </si>
-  <si>
     <t>B 1 21/d 1</t>
   </si>
   <si>
@@ -1173,9 +1170,6 @@
     <t>C 1 1 21, C 1 1 21/m</t>
   </si>
   <si>
-    <t>A 1 1 2, A 1 1 m, C 1 2/m 1</t>
-  </si>
-  <si>
     <t>A 1 1 a, A 1 2/a 1</t>
   </si>
   <si>
@@ -1203,7 +1197,85 @@
     <t>C 1 1 a, C 1 1 2/a</t>
   </si>
   <si>
-    <t>7, 15</t>
+    <t>B 1 d 1, B 1 2/d 1</t>
+  </si>
+  <si>
+    <t>B 1 21/a 1</t>
+  </si>
+  <si>
+    <t>A 1 1 2, A 1 1 m, A 1 2/m 1</t>
+  </si>
+  <si>
+    <t>gamma != 90</t>
+  </si>
+  <si>
+    <t>P 2 1 1, P m 1 1, P 2/m 1 1</t>
+  </si>
+  <si>
+    <t>P 21 1 1, P 21/m 1 1</t>
+  </si>
+  <si>
+    <t>P b 1 1, P 2/b 1 1</t>
+  </si>
+  <si>
+    <t>P c  1 1, P 2/c 1 1</t>
+  </si>
+  <si>
+    <t>P n 1 1, P 2/n 1 1</t>
+  </si>
+  <si>
+    <t>P 21/b 1 1</t>
+  </si>
+  <si>
+    <t>P 21/c 1 1</t>
+  </si>
+  <si>
+    <t>P 21/n 1 1</t>
+  </si>
+  <si>
+    <t>A 2 1 1, A m 1 1, A 2/m 1 1</t>
+  </si>
+  <si>
+    <t>A 21 1 1, A 21/m 1 1</t>
+  </si>
+  <si>
+    <t>A b 1 1, A 2/b 1 1</t>
+  </si>
+  <si>
+    <t>A d 1 1, A 2/d 1 1</t>
+  </si>
+  <si>
+    <t>k + l = 4n</t>
+  </si>
+  <si>
+    <t>A 21/a 1 1</t>
+  </si>
+  <si>
+    <t>A 21/d 1 1</t>
+  </si>
+  <si>
+    <t>B 2 1 1, B m 1 1, B 2/m 1 1</t>
+  </si>
+  <si>
+    <t>B b 1 1, B 2/b 1 1</t>
+  </si>
+  <si>
+    <t>C 2 1 1, C m 1 1, C 2/m 1 1</t>
+  </si>
+  <si>
+    <t>C c 1 1, C 2/c 1 1</t>
+  </si>
+  <si>
+    <t>I 2 1 1, I m 1 1, I 2/m 1 1</t>
+  </si>
+  <si>
+    <t>I b 1 1, I 2/b 1 1</t>
+  </si>
+  <si>
+    <t>F 2 1 1, F m 1 1, F 2/m 1 1</t>
+  </si>
+  <si>
+    <t>F d 1 1, F 2/d 1 1</t>
   </si>
 </sst>
 </file>
@@ -1697,17 +1769,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F97899-3E7B-2A4E-8106-D9711D155142}">
-  <dimension ref="A1:Q146"/>
+  <dimension ref="A1:Q220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D156" sqref="D156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -2065,13 +2137,13 @@
         <v>350</v>
       </c>
       <c r="J25" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="P25" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
@@ -2356,18 +2428,18 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D36" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
@@ -2468,18 +2540,18 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>357</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D46" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
@@ -2580,18 +2652,18 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>359</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D56" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -2694,18 +2766,18 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>362</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D66" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -2713,13 +2785,13 @@
         <v>1</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -2809,15 +2881,15 @@
     <row r="74" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="75" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="12" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>365</v>
+      </c>
+      <c r="D76" t="s">
         <v>366</v>
-      </c>
-      <c r="D76" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -2902,22 +2974,22 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>368</v>
+      </c>
+      <c r="D87" t="s">
+        <v>367</v>
+      </c>
+      <c r="G87" t="s">
         <v>369</v>
       </c>
-      <c r="D87" t="s">
-        <v>368</v>
-      </c>
-      <c r="G87" t="s">
+      <c r="J87" t="s">
+        <v>371</v>
+      </c>
+      <c r="M87" t="s">
         <v>370</v>
       </c>
-      <c r="J87" t="s">
+      <c r="P87" t="s">
         <v>372</v>
-      </c>
-      <c r="M87" t="s">
-        <v>371</v>
-      </c>
-      <c r="P87" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
@@ -3157,22 +3229,22 @@
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="D98" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="D98" s="3" t="s">
-        <v>378</v>
-      </c>
       <c r="G98" s="3" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="J98" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="M98" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="M98" s="3" t="s">
-        <v>387</v>
-      </c>
       <c r="P98" s="3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
@@ -3183,7 +3255,7 @@
         <v>339</v>
       </c>
       <c r="G99" t="s">
-        <v>389</v>
+        <v>341</v>
       </c>
       <c r="J99" t="s">
         <v>341</v>
@@ -3332,7 +3404,7 @@
         <v>4</v>
       </c>
       <c r="K103" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="M103" s="3" t="s">
         <v>4</v>
@@ -3344,7 +3416,7 @@
         <v>4</v>
       </c>
       <c r="Q103" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
@@ -3457,18 +3529,18 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="D108" s="3" t="s">
         <v>374</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D109" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
@@ -3569,18 +3641,18 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D119" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -3681,18 +3753,18 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D129" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -3795,18 +3867,18 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D139" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -3814,13 +3886,13 @@
         <v>1</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -3905,6 +3977,1106 @@
       </c>
       <c r="E146" s="3" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="12" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>391</v>
+      </c>
+      <c r="D150" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>337</v>
+      </c>
+      <c r="D151" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B152" s="3"/>
+      <c r="D152" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E152" s="3"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B153" s="3"/>
+      <c r="D153" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E153" s="3"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B154" s="3"/>
+      <c r="D154" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E154" s="3"/>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B155" s="3"/>
+      <c r="D155" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E155" s="3"/>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B156" s="3"/>
+      <c r="D156" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B157" s="3"/>
+      <c r="D157" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E157" s="3"/>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B158" s="3"/>
+      <c r="D158" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E158" s="3"/>
+    </row>
+    <row r="161" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>393</v>
+      </c>
+      <c r="D161" t="s">
+        <v>394</v>
+      </c>
+      <c r="G161" t="s">
+        <v>395</v>
+      </c>
+      <c r="J161" t="s">
+        <v>396</v>
+      </c>
+      <c r="M161" t="s">
+        <v>397</v>
+      </c>
+      <c r="P161" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="162" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>341</v>
+      </c>
+      <c r="D162" t="s">
+        <v>341</v>
+      </c>
+      <c r="G162" t="s">
+        <v>341</v>
+      </c>
+      <c r="J162">
+        <v>14</v>
+      </c>
+      <c r="M162">
+        <v>14</v>
+      </c>
+      <c r="P162">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="163" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A163" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B163" s="3"/>
+      <c r="D163" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E163" s="3"/>
+      <c r="G163" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H163" s="3"/>
+      <c r="J163" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K163" s="3"/>
+      <c r="M163" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N163" s="3"/>
+      <c r="P163" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q163" s="3"/>
+    </row>
+    <row r="164" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A164" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G164" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H164" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J164" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K164" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M164" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N164" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P164" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q164" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="165" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A165" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B165" s="3"/>
+      <c r="D165" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E165" s="3"/>
+      <c r="G165" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H165" s="3"/>
+      <c r="J165" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K165" s="3"/>
+      <c r="M165" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P165" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q165" s="3"/>
+    </row>
+    <row r="166" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A166" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B166" s="3"/>
+      <c r="D166" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E166" s="3"/>
+      <c r="G166" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H166" s="3"/>
+      <c r="J166" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K166" s="3"/>
+      <c r="M166" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N166" s="3"/>
+      <c r="P166" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q166" s="3"/>
+    </row>
+    <row r="167" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A167" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B167" s="3"/>
+      <c r="D167" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E167" s="3"/>
+      <c r="G167" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H167" s="3"/>
+      <c r="J167" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K167" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M167" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N167" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P167" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q167" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="168" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A168" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E168" s="3"/>
+      <c r="G168" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H168" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J168" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K168" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M168" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N168" s="3"/>
+      <c r="P168" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q168" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="169" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A169" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B169" s="3"/>
+      <c r="D169" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G169" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H169" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J169" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K169" s="3"/>
+      <c r="M169" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N169" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P169" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q169" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="172" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A172" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="G172" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="J172" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="M172" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="P172" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="173" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>337</v>
+      </c>
+      <c r="D173" t="s">
+        <v>339</v>
+      </c>
+      <c r="G173" t="s">
+        <v>341</v>
+      </c>
+      <c r="J173" t="s">
+        <v>341</v>
+      </c>
+      <c r="M173">
+        <v>14</v>
+      </c>
+      <c r="P173">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="174" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A174" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G174" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H174" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J174" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K174" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M174" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N174" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P174" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q174" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="175" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A175" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G175" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H175" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J175" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K175" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="M175" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N175" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P175" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q175" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="176" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A176" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G176" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H176" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J176" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K176" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M176" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N176" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P176" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q176" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="177" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A177" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G177" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H177" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J177" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K177" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M177" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N177" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P177" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q177" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="178" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A178" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B178" s="3"/>
+      <c r="D178" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G178" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H178" s="3"/>
+      <c r="J178" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K178" s="3"/>
+      <c r="M178" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N178" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P178" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q178" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="179" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A179" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G179" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H179" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J179" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K179" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M179" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N179" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P179" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q179" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="180" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A180" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G180" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H180" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J180" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K180" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M180" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N180" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P180" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q180" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="182" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A182" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="D182" s="3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="183" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>353</v>
+      </c>
+      <c r="D183" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="184" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A184" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="185" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A185" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="186" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A186" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="187" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A187" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="188" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A188" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="189" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A189" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B189" s="3"/>
+      <c r="D189" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="190" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A190" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="192" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A192" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>353</v>
+      </c>
+      <c r="D193" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A194" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A195" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E195" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D198" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E198" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E199" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B200" s="3"/>
+      <c r="D200" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A202" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>353</v>
+      </c>
+      <c r="D203" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A204" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A205" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D205" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E205" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A207" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A208" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D208" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E208" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D210" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="D212" s="3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>353</v>
+      </c>
+      <c r="D213" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E214" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D215" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E215" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D216" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E216" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D217" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E217" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D218" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E218" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D219" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E219" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E220" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added check for off by two and spacegroup assignment
</commit_message>
<xml_diff>
--- a/data/SpacegroupGroups.xlsx
+++ b/data/SpacegroupGroups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DWMoreau/MLI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB744384-3652-714A-93F9-070D669F4890}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771EAD14-6674-3B4A-8D46-3AE98349EFB9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="800" windowWidth="25300" windowHeight="17800" activeTab="2" xr2:uid="{858AA173-3D70-D14E-A9ED-F265E8D33CB5}"/>
+    <workbookView xWindow="2540" yWindow="760" windowWidth="25300" windowHeight="17760" activeTab="2" xr2:uid="{858AA173-3D70-D14E-A9ED-F265E8D33CB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Monoclinic, beta" sheetId="10" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5000" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5001" uniqueCount="446">
   <si>
     <t>F222</t>
   </si>
@@ -848,12 +848,6 @@
     <t>h, k = 2n, h + k = 4n</t>
   </si>
   <si>
-    <t>F 2 3, F m 3, F 4 3 2</t>
-  </si>
-  <si>
-    <t>196, 202, 209</t>
-  </si>
-  <si>
     <t>F 41 3 2</t>
   </si>
   <si>
@@ -878,39 +872,21 @@
     <t>P 2 3, P m -3, P432, P -43n, P m -3 m, P -4 3 m</t>
   </si>
   <si>
-    <t>195, 200, 207, 218, 221, 215</t>
-  </si>
-  <si>
     <t>P 42/n</t>
   </si>
   <si>
     <t>I 41/a</t>
   </si>
   <si>
-    <t>P 41, P 42, P 42/m, P 42 2 2</t>
-  </si>
-  <si>
-    <t>76, 77, 84, 93</t>
-  </si>
-  <si>
     <t>P 42 21 2</t>
   </si>
   <si>
-    <t>P 43, P 41 2 2, P 43 2 2</t>
-  </si>
-  <si>
-    <t>78, 91, 95</t>
-  </si>
-  <si>
     <t>I 41, I 41 2 2</t>
   </si>
   <si>
     <t>80, 98</t>
   </si>
   <si>
-    <t>P 42 c m</t>
-  </si>
-  <si>
     <t>2h + l = 4n</t>
   </si>
   <si>
@@ -989,12 +965,6 @@
     <t>105, 112, 131</t>
   </si>
   <si>
-    <t>P -4 c 2, P 42/m c m</t>
-  </si>
-  <si>
-    <t>116, 132</t>
-  </si>
-  <si>
     <t>P 42/n b c</t>
   </si>
   <si>
@@ -1340,9 +1310,6 @@
     <t>173, 176, 182</t>
   </si>
   <si>
-    <t>186, 190</t>
-  </si>
-  <si>
     <t>P6, P -6, P 6/m, P 6 2 2, P 6 m m, P -6 m 2, P -6 2 m, P 6/mmm</t>
   </si>
   <si>
@@ -1362,6 +1329,51 @@
   </si>
   <si>
     <t>P 63 m c, P -6 2 c, P 63/mmc</t>
+  </si>
+  <si>
+    <t>F 4 3 2</t>
+  </si>
+  <si>
+    <t>F d -3</t>
+  </si>
+  <si>
+    <t>195, 200, 207, 215, 221</t>
+  </si>
+  <si>
+    <t>186, 190, 194</t>
+  </si>
+  <si>
+    <t>same but miss labeled here</t>
+  </si>
+  <si>
+    <t>77, 84, 93</t>
+  </si>
+  <si>
+    <t>76, 78, 91, 95</t>
+  </si>
+  <si>
+    <t>P 42, P 42/m, P 42 2 2</t>
+  </si>
+  <si>
+    <t>P 41, P 43, P 41 2 2, P 43 2 2</t>
+  </si>
+  <si>
+    <t>same but not correctly labeled</t>
+  </si>
+  <si>
+    <t>209, 216, 225</t>
+  </si>
+  <si>
+    <t>203, 227</t>
+  </si>
+  <si>
+    <t>101, 116, 132</t>
+  </si>
+  <si>
+    <t>P 42 c m, P -4 c 2, P 42/m c m</t>
+  </si>
+  <si>
+    <t>Same but incorrect here:</t>
   </si>
 </sst>
 </file>
@@ -1857,31 +1869,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F97899-3E7B-2A4E-8106-D9711D155142}">
   <dimension ref="A1:Q220"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D156" sqref="D156"/>
+    <sheetView topLeftCell="A82" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="D3" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="D4" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -1958,33 +1970,33 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="D14" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="G14" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="J14" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="M14" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="P14" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="D15" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="G15" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="J15">
         <v>14</v>
@@ -2214,36 +2226,36 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="D26" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="G26" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="J26" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="M26">
         <v>14</v>
@@ -2351,7 +2363,7 @@
         <v>3</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="M29" s="3" t="s">
         <v>3</v>
@@ -2363,7 +2375,7 @@
         <v>3</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
@@ -2514,18 +2526,18 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D36" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
@@ -2626,18 +2638,18 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D46" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
@@ -2738,18 +2750,18 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D56" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -2852,18 +2864,18 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D66" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -2871,13 +2883,13 @@
         <v>1</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -2967,23 +2979,23 @@
     <row r="74" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="75" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="12" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="D76" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="D77" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -3060,33 +3072,33 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="D87" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="G87" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="J87" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="M87" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="P87" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="D88" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="G88" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="J88">
         <v>14</v>
@@ -3315,36 +3327,36 @@
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="G98" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="D98" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="G98" s="3" t="s">
-        <v>386</v>
-      </c>
       <c r="J98" s="3" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="M98" s="3" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="P98" s="3" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="D99" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="G99" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="J99" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="M99">
         <v>14</v>
@@ -3490,7 +3502,7 @@
         <v>4</v>
       </c>
       <c r="K103" s="3" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="M103" s="3" t="s">
         <v>4</v>
@@ -3502,7 +3514,7 @@
         <v>4</v>
       </c>
       <c r="Q103" s="3" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
@@ -3615,18 +3627,18 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D109" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
@@ -3727,18 +3739,18 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D119" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -3839,18 +3851,18 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D129" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -3953,18 +3965,18 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D139" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -3972,13 +3984,13 @@
         <v>1</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -4067,23 +4079,23 @@
     </row>
     <row r="149" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A149" s="12" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="D150" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="D151" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -4160,33 +4172,33 @@
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="D161" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="G161" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="J161" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="M161" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="P161" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="D162" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="G162" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="J162">
         <v>14</v>
@@ -4415,36 +4427,36 @@
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="J172" s="3" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="M172" s="3" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="P172" s="3" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="D173" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="G173" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="J173" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="M173">
         <v>14</v>
@@ -4514,7 +4526,7 @@
         <v>2</v>
       </c>
       <c r="K175" s="3" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="M175" s="3" t="s">
         <v>2</v>
@@ -4526,7 +4538,7 @@
         <v>2</v>
       </c>
       <c r="Q175" s="3" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
@@ -4715,18 +4727,18 @@
     </row>
     <row r="182" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
     </row>
     <row r="183" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D183" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="184" spans="1:17" x14ac:dyDescent="0.2">
@@ -4827,18 +4839,18 @@
     </row>
     <row r="192" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D193" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
@@ -4939,18 +4951,18 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D203" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
@@ -5053,18 +5065,18 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D213" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
@@ -5072,13 +5084,13 @@
         <v>1</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E214" s="3" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
@@ -9474,15 +9486,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A07B9D3-5C67-AB41-9F60-D3C009703861}">
-  <dimension ref="A1:J94"/>
+  <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>35</v>
       </c>
@@ -9495,8 +9507,11 @@
         <v>37</v>
       </c>
       <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>20</v>
       </c>
@@ -9509,8 +9524,9 @@
         <v>20</v>
       </c>
       <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -9535,8 +9551,10 @@
       <c r="J3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -9561,8 +9579,10 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -9588,7 +9608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -9607,8 +9627,10 @@
       <c r="H6" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L6" s="9"/>
+      <c r="N6" s="9"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -9627,8 +9649,10 @@
       <c r="H7" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L7" s="9"/>
+      <c r="N7" s="9"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -9647,8 +9671,10 @@
       <c r="H8" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L8" s="9"/>
+      <c r="N8" s="9"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -9668,7 +9694,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>49</v>
       </c>
@@ -9681,7 +9707,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>50</v>
       </c>
@@ -9694,7 +9720,7 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>1</v>
       </c>
@@ -9720,7 +9746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>2</v>
       </c>
@@ -9746,7 +9772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>3</v>
       </c>
@@ -9772,7 +9798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>4</v>
       </c>
@@ -11822,20 +11848,20 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="B2" s="3"/>
     </row>
@@ -11883,13 +11909,13 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="B12" s="3"/>
     </row>
@@ -11954,29 +11980,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7CB1F6-6441-6942-BBD8-72BEF197CCBA}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="B1" s="3"/>
       <c r="G1" s="3" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="B2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="H2" s="3"/>
     </row>
@@ -12052,21 +12078,21 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="B12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="B13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="H13" s="3"/>
     </row>
@@ -12135,32 +12161,32 @@
         <v>7</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="B23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="B24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="H24" s="3"/>
     </row>
@@ -12239,26 +12265,26 @@
         <v>7</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="B34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="B35" s="3"/>
       <c r="G35" s="3" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="H35" s="3"/>
     </row>
@@ -12346,17 +12372,17 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G44" s="3" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="H44" s="3"/>
       <c r="J44" s="3" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="K44" s="3"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G45" s="3" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
       <c r="H45" s="3"/>
       <c r="J45" s="3" t="s">
@@ -12458,13 +12484,13 @@
     </row>
     <row r="55" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G55" s="3" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="H55" s="3"/>
     </row>
     <row r="56" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G56" s="3" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="H56" s="3"/>
     </row>
@@ -15746,23 +15772,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3512D7-A514-8E4F-BD6D-507969E8403F}">
-  <dimension ref="A1:N79"/>
+  <dimension ref="A1:R79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="A1:B9"/>
+      <selection activeCell="R40" sqref="R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>280</v>
+        <v>433</v>
       </c>
       <c r="B2" s="3"/>
     </row>
@@ -16005,7 +16031,7 @@
         <v>246</v>
       </c>
       <c r="M19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -16110,7 +16136,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -16118,7 +16144,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>240</v>
       </c>
@@ -16126,7 +16152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>241</v>
       </c>
@@ -16134,7 +16160,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>242</v>
       </c>
@@ -16142,7 +16168,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>256</v>
       </c>
@@ -16158,8 +16184,11 @@
       <c r="M39" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P39" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>257</v>
       </c>
@@ -16175,8 +16204,14 @@
       <c r="M40" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P40" t="s">
+        <v>257</v>
+      </c>
+      <c r="R40" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>1</v>
       </c>
@@ -16205,7 +16240,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>2</v>
       </c>
@@ -16237,7 +16272,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>3</v>
       </c>
@@ -16269,7 +16304,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>4</v>
       </c>
@@ -16301,7 +16336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>5</v>
       </c>
@@ -16327,7 +16362,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>6</v>
       </c>
@@ -16353,7 +16388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>7</v>
       </c>
@@ -16379,7 +16414,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="G48" s="3" t="s">
         <v>240</v>
       </c>
@@ -16393,7 +16428,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="G49" s="3" t="s">
         <v>241</v>
       </c>
@@ -16407,7 +16442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="G50" s="3" t="s">
         <v>242</v>
       </c>
@@ -16421,35 +16456,38 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>265</v>
       </c>
       <c r="E52" t="s">
+        <v>431</v>
+      </c>
+      <c r="I52" t="s">
+        <v>432</v>
+      </c>
+      <c r="M52" t="s">
         <v>270</v>
       </c>
-      <c r="I52" t="s">
-        <v>265</v>
-      </c>
-      <c r="M52" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>266</v>
       </c>
-      <c r="E53" t="s">
-        <v>271</v>
-      </c>
-      <c r="I53" t="s">
-        <v>266</v>
+      <c r="E53">
+        <v>209</v>
+      </c>
+      <c r="I53">
+        <v>203</v>
       </c>
       <c r="M53">
         <v>210</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q53" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>1</v>
       </c>
@@ -16474,8 +16512,14 @@
       <c r="N54" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q54" t="s">
+        <v>266</v>
+      </c>
+      <c r="R54" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>2</v>
       </c>
@@ -16500,8 +16544,11 @@
       <c r="N55" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q55" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>3</v>
       </c>
@@ -16527,7 +16574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>4</v>
       </c>
@@ -16553,7 +16600,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>5</v>
       </c>
@@ -16579,7 +16626,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>6</v>
       </c>
@@ -16605,7 +16652,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>7</v>
       </c>
@@ -16631,7 +16678,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E61" s="3" t="s">
         <v>240</v>
       </c>
@@ -16645,7 +16692,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E62" s="3" t="s">
         <v>241</v>
       </c>
@@ -16659,7 +16706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E63" s="3" t="s">
         <v>242</v>
       </c>
@@ -16675,24 +16722,24 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>271</v>
+      </c>
+      <c r="E65" t="s">
         <v>273</v>
       </c>
-      <c r="E65" t="s">
+      <c r="I65" t="s">
         <v>275</v>
       </c>
-      <c r="I65" t="s">
-        <v>277</v>
-      </c>
       <c r="M65" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>272</v>
+      </c>
+      <c r="E66" t="s">
         <v>274</v>
-      </c>
-      <c r="E66" t="s">
-        <v>276</v>
       </c>
       <c r="I66">
         <v>227</v>
@@ -17049,32 +17096,35 @@
   <dimension ref="A1:Q90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B10"/>
+      <selection activeCell="P3" sqref="P2:Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B1" s="3"/>
       <c r="F1" s="3" t="s">
-        <v>283</v>
+        <v>438</v>
       </c>
       <c r="G1" s="3"/>
       <c r="I1" s="3" t="s">
-        <v>286</v>
+        <v>439</v>
       </c>
       <c r="J1" s="3"/>
       <c r="L1" s="3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B2" s="3"/>
       <c r="F2" s="3"/>
@@ -17083,26 +17133,30 @@
       <c r="J2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>284</v>
+        <v>436</v>
       </c>
       <c r="G3" s="3"/>
       <c r="I3" s="3" t="s">
-        <v>287</v>
+        <v>437</v>
       </c>
       <c r="J3" s="3"/>
       <c r="L3" s="3">
         <v>94</v>
       </c>
       <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -17120,7 +17174,7 @@
       </c>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -17138,7 +17192,7 @@
       </c>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -17156,7 +17210,7 @@
       </c>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -17174,7 +17228,7 @@
       </c>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -17194,7 +17248,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -17214,7 +17268,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -17238,31 +17292,31 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="H12" s="3"/>
       <c r="J12" s="3" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="K12" s="3"/>
       <c r="M12" s="3" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B13" s="3"/>
       <c r="D13" s="3">
@@ -17270,11 +17324,11 @@
       </c>
       <c r="E13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="H13" s="3"/>
       <c r="J13" s="3" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="K13" s="3"/>
       <c r="M13" s="3">
@@ -17282,7 +17336,7 @@
       </c>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -17304,7 +17358,7 @@
       </c>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -17328,7 +17382,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>3</v>
       </c>
@@ -17472,45 +17526,41 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="D22" s="3" t="s">
-        <v>290</v>
-      </c>
+      <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="H22" s="3"/>
       <c r="J22" s="3" t="s">
-        <v>317</v>
+        <v>444</v>
       </c>
       <c r="K22" s="3"/>
       <c r="M22" s="3" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="N22" s="3"/>
       <c r="P22" s="3" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="Q22" s="3"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="D23" s="3">
-        <v>101</v>
-      </c>
+      <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="H23" s="3"/>
       <c r="J23" s="3" t="s">
-        <v>318</v>
+        <v>443</v>
       </c>
       <c r="K23" s="3"/>
       <c r="M23" s="3">
@@ -17527,9 +17577,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="D24" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="G24" s="3" t="s">
         <v>1</v>
@@ -17555,12 +17603,8 @@
       <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
       <c r="G25" s="3" t="s">
         <v>2</v>
       </c>
@@ -17593,9 +17637,7 @@
       <c r="B26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="G26" s="3" t="s">
         <v>3</v>
@@ -17627,9 +17669,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="3"/>
-      <c r="D27" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="G27" s="3" t="s">
         <v>4</v>
@@ -17659,9 +17699,7 @@
       <c r="B28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="G28" s="3" t="s">
         <v>5</v>
@@ -17693,9 +17731,7 @@
       <c r="B29" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="G29" s="3" t="s">
         <v>6</v>
@@ -17725,12 +17761,8 @@
         <v>7</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="D30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
       <c r="G30" s="3" t="s">
         <v>7</v>
       </c>
@@ -17758,41 +17790,41 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="B32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="E32" s="3"/>
       <c r="G32" s="3" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="H32" s="3"/>
       <c r="J32" s="3" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="K32" s="3"/>
       <c r="M32" s="3" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E33" s="3"/>
       <c r="G33" s="3" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="H33" s="3"/>
       <c r="J33" s="3" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="K33" s="3"/>
       <c r="M33" s="3">
@@ -17903,7 +17935,7 @@
         <v>4</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
@@ -18028,19 +18060,19 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="B43" s="3"/>
       <c r="D43" s="3" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="E43" s="3"/>
       <c r="G43" s="3" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="H43" s="3"/>
       <c r="J43" s="3" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="K43" s="3"/>
     </row>
@@ -18148,7 +18180,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>5</v>
       </c>
@@ -18174,7 +18206,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>6</v>
       </c>
@@ -18200,7 +18232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>7</v>
       </c>
@@ -18226,7 +18258,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>245</v>
       </c>
@@ -18252,26 +18284,29 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="G57" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="M57" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>289</v>
+      </c>
+      <c r="D58" t="s">
         <v>282</v>
-      </c>
-      <c r="J57" s="3" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>297</v>
-      </c>
-      <c r="D58" t="s">
-        <v>289</v>
       </c>
       <c r="G58">
         <v>88</v>
@@ -18279,8 +18314,14 @@
       <c r="J58">
         <v>120</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M58" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="O58" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>1</v>
       </c>
@@ -18306,7 +18347,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>2</v>
       </c>
@@ -18331,8 +18372,14 @@
       <c r="K60" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M60" t="s">
+        <v>321</v>
+      </c>
+      <c r="O60">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>3</v>
       </c>
@@ -18358,7 +18405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>4</v>
       </c>
@@ -18384,7 +18431,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>5</v>
       </c>
@@ -18410,7 +18457,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>6</v>
       </c>
@@ -18464,27 +18511,27 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="D69" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="G69" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="J69">
         <v>110</v>
@@ -18689,13 +18736,13 @@
         <v>245</v>
       </c>
       <c r="H77" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="J77" s="3" t="s">
         <v>245</v>
       </c>
       <c r="K77" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -18714,10 +18761,10 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G80" s="3" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="81" spans="7:11" x14ac:dyDescent="0.2">
@@ -18831,13 +18878,13 @@
         <v>245</v>
       </c>
       <c r="H89" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="J89" s="3" t="s">
         <v>245</v>
       </c>
       <c r="K89" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="90" spans="7:11" x14ac:dyDescent="0.2">
@@ -20394,7 +20441,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>